<commit_message>
* Finished thesis algorithms * Run benchmark on thesis algorithms * Prepared latex code samples * Included latex code samples in latex
</commit_message>
<xml_diff>
--- a/results/2013_08_09_sort_bitonic_high_res.xlsx
+++ b/results/2013_08_09_sort_bitonic_high_res.xlsx
@@ -4486,11 +4486,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99240768"/>
-        <c:axId val="76774144"/>
+        <c:axId val="54923200"/>
+        <c:axId val="54923776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99240768"/>
+        <c:axId val="54923200"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4527,12 +4527,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76774144"/>
+        <c:crossAx val="54923776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76774144"/>
+        <c:axId val="54923776"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4563,7 +4563,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99240768"/>
+        <c:crossAx val="54923200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4909,8 +4909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J630"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E161" sqref="E161"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>